<commit_message>
Update switch matrix geo file
</commit_message>
<xml_diff>
--- a/maps/SwitchBoardMapping.xlsx
+++ b/maps/SwitchBoardMapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10845"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10845" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maps" sheetId="3" r:id="rId1"/>
@@ -365,27 +365,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -768,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K606"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -13446,8 +13426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15079,7 +15059,7 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P33">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16204,10 +16184,10 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P22 A33:P33 A23:I32 K23:P32">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17327,7 +17307,7 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P33">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18515,7 +18495,7 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P33">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18526,7 +18506,7 @@
   <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19458,10 +19438,10 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:P33">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:B48">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new HexPlot version, add possibility for sensor specific corr files
</commit_message>
<xml_diff>
--- a/maps/SwitchBoardMapping.xlsx
+++ b/maps/SwitchBoardMapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
     <sheet name="Maps" sheetId="3" r:id="rId1"/>
     <sheet name="Switch card" sheetId="1" r:id="rId2"/>
     <sheet name="Probe card HPK 6in" sheetId="2" r:id="rId3"/>
-    <sheet name="Probe card HPK 6in 265cells" sheetId="6" r:id="rId4"/>
+    <sheet name="Probe card HPK 6in 256cells" sheetId="6" r:id="rId4"/>
     <sheet name="Probe card HPK 8in" sheetId="4" r:id="rId5"/>
     <sheet name="Probe card IFX 8in" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -710,9 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K270" sqref="K270"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -739,8 +739,8 @@
         <v>Probe card IFX 8in</v>
       </c>
       <c r="E1" s="18" t="str">
-        <f ca="1">'Probe card HPK 6in 265cells'!$A$1</f>
-        <v>Probe card HPK 6in 265cells</v>
+        <f ca="1">'Probe card HPK 6in 256cells'!$A$1</f>
+        <v>Probe card HPK 6in 256cells</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="19" customFormat="1" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
@@ -754,15 +754,15 @@
       </c>
       <c r="C2" s="19">
         <f ca="1">SUMPRODUCT(NOT(ISBLANK(C$3:C$1000))*1)-COUNTIF(C$3:C$1000,"=#VALUE!")</f>
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D2" s="19">
         <f ca="1">SUMPRODUCT(NOT(ISBLANK(D$3:D$1000))*1)-COUNTIF(D$3:D$1000,"=#VALUE!")</f>
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E2" s="19">
         <f ca="1">SUMPRODUCT(NOT(ISBLANK(E$3:E$1000))*1)-COUNTIF(E$3:E$1000,"=#VALUE!")</f>
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -5766,7 +5766,7 @@
       </c>
       <c r="D240" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A240)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A240)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E240" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A240)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A240)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="D241" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A241)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A241)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E241" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A241)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A241)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -5808,11 +5808,11 @@
       </c>
       <c r="D242" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A242)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A242)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E242" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A242)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A242)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.45">
@@ -5829,11 +5829,11 @@
       </c>
       <c r="D243" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A243)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A243)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E243" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A243)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A243)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.45">
@@ -5850,11 +5850,11 @@
       </c>
       <c r="D244" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A244)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A244)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E244" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A244)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A244)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.45">
@@ -5871,11 +5871,11 @@
       </c>
       <c r="D245" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A245)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A245)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E245" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A245)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A245)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.45">
@@ -5892,11 +5892,11 @@
       </c>
       <c r="D246" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A246)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A246)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E246" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A246)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A246)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.45">
@@ -5913,11 +5913,11 @@
       </c>
       <c r="D247" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A247)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A247)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E247" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A247)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A247)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.45">
@@ -5932,13 +5932,13 @@
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A248)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A248)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
         <v>368</v>
       </c>
-      <c r="D248" s="21" t="e">
+      <c r="D248" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A248)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A248)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>#VALUE!</v>
+        <v>14</v>
       </c>
       <c r="E248" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A248)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A248)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.45">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="E249" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A249)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A249)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.45">
@@ -5978,9 +5978,9 @@
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A250)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A250)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E250" s="21" t="e">
+      <c r="E250" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A250)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A250)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>#VALUE!</v>
+        <v>14</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.45">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="C274" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A274)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A274)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D274" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A274)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A274)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6497,7 +6497,7 @@
       </c>
       <c r="C275" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A275)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A275)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D275" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A275)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A275)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="C276" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A276)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A276)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D276" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A276)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A276)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="C277" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A277)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A277)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D277" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A277)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A277)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6560,7 +6560,7 @@
       </c>
       <c r="C278" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A278)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A278)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D278" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A278)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A278)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="C279" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A279)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A279)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D279" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A279)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A279)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6602,7 +6602,7 @@
       </c>
       <c r="C280" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A280)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A280)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D280" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A280)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A280)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="C281" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A281)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A281)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D281" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A281)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A281)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -6642,9 +6642,9 @@
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;B$1&amp;"'!$A$1:$P$33")=$A282)*ROW(INDIRECT("'"&amp;B$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;B$1&amp;"'!$A$1:$P$33")=$A282)*COLUMN(INDIRECT("'"&amp;B$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C282" s="21" t="e">
+      <c r="C282" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A282)*ROW(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33")=$A282)*COLUMN(INDIRECT("'"&amp;C$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>#VALUE!</v>
+        <v>14</v>
       </c>
       <c r="D282" s="21" t="e">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A282)*ROW(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33")=$A282)*COLUMN(INDIRECT("'"&amp;D$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
@@ -13370,6 +13370,7 @@
       <c r="B606" s="21"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13380,7 +13381,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15970,7 +15971,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15978,7 +15979,7 @@
     <row r="1" spans="1:16" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
-        <v>Probe card HPK 6in 265cells</v>
+        <v>Probe card HPK 6in 256cells</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -15998,7 +15999,7 @@
     </row>
     <row r="2" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -16018,7 +16019,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="4"/>
@@ -16038,7 +16039,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="4"/>
@@ -16058,7 +16059,7 @@
     </row>
     <row r="5" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="6">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="6"/>
@@ -16078,7 +16079,7 @@
     </row>
     <row r="6" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -16098,7 +16099,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
@@ -16118,7 +16119,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
@@ -16138,7 +16139,7 @@
     </row>
     <row r="9" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="7">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
@@ -17014,7 +17015,9 @@
       <c r="A33" s="15">
         <v>157</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="16">
+        <v>240</v>
+      </c>
       <c r="C33" s="15">
         <v>159</v>
       </c>
@@ -17075,10 +17078,10 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A33:P33 A23:I32 K23:P32 A18:P22 C14:P17 A1:P13">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:XFD1048576 C14:XFD17 A1:XFD13">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17089,7 +17092,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17117,7 +17120,7 @@
     </row>
     <row r="2" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="11"/>
@@ -17137,7 +17140,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -17157,7 +17160,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="13">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="13"/>
@@ -17177,7 +17180,7 @@
     </row>
     <row r="5" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="15">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="15"/>
@@ -17196,8 +17199,8 @@
       <c r="P5" s="16"/>
     </row>
     <row r="6" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="12">
-        <v>276</v>
+      <c r="A6" s="11">
+        <v>277</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
@@ -17216,8 +17219,8 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="14">
-        <v>277</v>
+      <c r="A7" s="13">
+        <v>278</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="13"/>
@@ -17236,8 +17239,8 @@
       <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="14">
-        <v>278</v>
+      <c r="A8" s="13">
+        <v>279</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="13"/>
@@ -17256,8 +17259,8 @@
       <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="16">
-        <v>279</v>
+      <c r="A9" s="15">
+        <v>280</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="15"/>
@@ -18197,7 +18200,9 @@
       <c r="A33" s="15">
         <v>20</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="16">
+        <v>272</v>
+      </c>
       <c r="C33" s="15">
         <v>34</v>
       </c>
@@ -18258,7 +18263,7 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A18:P33 C14:P17 A1:P13">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18269,7 +18274,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18297,7 +18302,7 @@
     </row>
     <row r="2" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="11">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="11"/>
@@ -18317,7 +18322,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="13"/>
@@ -18337,7 +18342,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="13">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="13"/>
@@ -18357,7 +18362,7 @@
     </row>
     <row r="5" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="15">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="15"/>
@@ -18376,8 +18381,8 @@
       <c r="P5" s="16"/>
     </row>
     <row r="6" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="12">
-        <v>242</v>
+      <c r="A6" s="11">
+        <v>243</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="11"/>
@@ -18396,8 +18401,8 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="14">
-        <v>243</v>
+      <c r="A7" s="13">
+        <v>244</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="13"/>
@@ -18416,8 +18421,8 @@
       <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="14">
-        <v>244</v>
+      <c r="A8" s="13">
+        <v>245</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="13"/>
@@ -18436,8 +18441,8 @@
       <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="16">
-        <v>245</v>
+      <c r="A9" s="15">
+        <v>246</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="15"/>
@@ -19309,7 +19314,9 @@
       <c r="A33" s="15">
         <v>188</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="16">
+        <v>238</v>
+      </c>
       <c r="C33" s="15">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Corrected map for 6-inch 240-channel probe card
</commit_message>
<xml_diff>
--- a/maps/SwitchBoardMapping.xlsx
+++ b/maps/SwitchBoardMapping.xlsx
@@ -712,7 +712,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +783,7 @@
       </c>
       <c r="E3" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A3)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A3)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="E4" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A4)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A4)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>378</v>
+        <v>255</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="E5" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A5)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A5)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="E6" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A6)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A6)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="E7" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A7)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A7)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>383</v>
+        <v>250</v>
       </c>
       <c r="F7" s="22"/>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="E8" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A8)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A8)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>291</v>
+        <v>234</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -918,7 +918,7 @@
       </c>
       <c r="E9" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A9)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A9)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>441</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
       </c>
       <c r="E10" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A10)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A10)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>191</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
       </c>
       <c r="E11" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A11)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A11)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>311</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
       </c>
       <c r="E12" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A12)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A12)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>420</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="E13" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A13)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A13)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>161</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="E14" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A14)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A14)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>364</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="E15" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A15)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A15)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>119</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="E16" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A16)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A16)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>495</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="E17" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A17)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A17)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>185</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="E18" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A18)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A18)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>428</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="E20" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A20)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A20)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>99</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="E21" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A21)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A21)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>368</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="E22" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A22)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A22)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>298</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="E23" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A23)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A23)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>167</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="E24" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A24)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A24)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="E25" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A25)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A25)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>360</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E26" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A26)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A26)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="E27" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A27)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A27)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>171</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E28" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A28)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A28)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>443</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="E29" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A29)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A29)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>190</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="E30" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A30)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A30)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>122</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E31" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A31)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A31)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>319</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="E32" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A32)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A32)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>438</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="E33" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A33)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A33)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>300</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="E34" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A34)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A34)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>310</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="E35" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A35)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A35)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>172</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E36" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A36)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A36)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>372</v>
+        <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="E37" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A37)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A37)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>511</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="E38" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A38)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A38)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="E39" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A39)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A39)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>247</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="E40" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A40)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A40)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>105</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="E41" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A41)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A41)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>318</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
       </c>
       <c r="E42" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A42)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A42)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>226</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="E43" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A43)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A43)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>422</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="E44" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A44)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A44)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>432</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="E45" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A45)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A45)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>183</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="E46" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A46)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A46)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>96</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="E47" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A47)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A47)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>184</v>
+        <v>446</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="E48" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A48)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A48)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>439</v>
+        <v>356</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="E49" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A49)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A49)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>113</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="E50" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A50)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A50)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>235</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="E51" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A51)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A51)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="E52" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A52)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A52)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>302</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="E53" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A53)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A53)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>255</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="E54" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A54)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A54)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="E55" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A55)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A55)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="E56" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A56)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A56)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>447</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="E57" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A57)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A57)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="E58" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A58)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A58)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>180</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="E59" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A59)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A59)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>423</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="E60" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A60)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A60)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>225</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="E61" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A61)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A61)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>309</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E62" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A62)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A62)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>181</v>
+        <v>381</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="E63" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A63)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A63)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>308</v>
+        <v>423</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E64" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A64)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A64)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>418</v>
+        <v>510</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="E65" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A65)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A65)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>293</v>
+        <v>442</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="E66" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A66)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A66)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="E67" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A67)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A67)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>377</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="E68" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A68)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A68)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>252</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="E69" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A69)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A69)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>440</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="E70" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A70)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A70)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="E71" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A71)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A71)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>434</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="E72" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A72)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A72)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>381</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="E73" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A73)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A73)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E74" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A74)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A74)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>125</v>
+        <v>305</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="E75" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A75)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A75)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>241</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="E76" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A76)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A76)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>173</v>
+        <v>307</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="E77" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A77)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A77)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>103</v>
+        <v>309</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="E78" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A78)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A78)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>382</v>
+        <v>444</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
       </c>
       <c r="E79" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A79)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A79)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E80" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A80)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A80)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="E81" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A81)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A81)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>234</v>
+        <v>433</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="E82" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A82)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A82)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="E83" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A83)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A83)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>188</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="E84" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A84)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A84)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>253</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="E85" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A85)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A85)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>101</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E86" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A86)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A86)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>186</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="E87" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A87)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A87)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>363</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="E88" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A88)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A88)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="E89" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A89)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A89)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="E90" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A90)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A90)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>354</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="E91" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A91)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A91)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>236</v>
+        <v>367</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
       </c>
       <c r="E92" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A92)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A92)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>307</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="E93" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A93)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A93)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>444</v>
+        <v>420</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="E94" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A94)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A94)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>178</v>
+        <v>441</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="E95" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A95)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A95)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>353</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="E96" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A96)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A96)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>312</v>
+        <v>434</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="E97" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A97)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A97)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>232</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="E98" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A98)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A98)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>371</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="E99" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A99)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A99)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>316</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="E100" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A100)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A100)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>446</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="E101" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A101)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A101)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>296</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,7 +2872,7 @@
       </c>
       <c r="E102" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A102)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A102)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>369</v>
+        <v>235</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="E103" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A103)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A103)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>123</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="E104" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A104)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A104)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>238</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="E105" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A105)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A105)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>115</v>
+        <v>253</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="E106" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A106)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A106)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>510</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="E107" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A107)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A107)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>249</v>
+        <v>369</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="E108" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A108)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A108)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>127</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="E109" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A109)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A109)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>295</v>
+        <v>352</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="E110" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A110)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A110)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>304</v>
+        <v>438</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E111" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A111)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A111)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>254</v>
+        <v>371</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="E112" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A112)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A112)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>433</v>
+        <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="E113" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A113)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A113)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>356</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
       </c>
       <c r="E114" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A114)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A114)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>297</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="E115" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A115)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A115)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>289</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="E116" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A116)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A116)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>250</v>
+        <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
       </c>
       <c r="E117" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A117)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A117)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>164</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="E118" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A118)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A118)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>102</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="E119" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A119)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A119)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>240</v>
+        <v>314</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="E120" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A120)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A120)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="E121" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A121)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A121)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>228</v>
+        <v>319</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E122" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A122)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A122)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>242</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="E123" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A123)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A123)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>442</v>
+        <v>382</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="E124" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A124)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A124)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>301</v>
+        <v>418</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,7 +3355,7 @@
       </c>
       <c r="E125" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A125)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A125)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>313</v>
+        <v>511</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="E126" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A126)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A126)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>362</v>
+        <v>495</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
       </c>
       <c r="E127" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A127)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A127)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>251</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E128" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A128)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A128)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>229</v>
+        <v>101</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
       </c>
       <c r="E129" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A129)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A129)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>163</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
       </c>
       <c r="E130" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A130)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A130)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>303</v>
+        <v>122</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="E131" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A131)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A131)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>374</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3502,7 +3502,7 @@
       </c>
       <c r="E132" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A132)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A132)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>315</v>
+        <v>177</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="E133" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A133)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A133)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
       </c>
       <c r="E134" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A134)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A134)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>314</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="E135" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A135)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A135)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>166</v>
+        <v>318</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="E136" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A136)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A136)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>352</v>
+        <v>364</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3607,7 +3607,7 @@
       </c>
       <c r="E137" s="21">
         <f ca="1">INDIRECT("'"&amp;'Switch card'!$A$1&amp;"'!"&amp;ADDRESS(SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A137)*ROW(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))),SUMPRODUCT((INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33")=$A137)*COLUMN(INDIRECT("'"&amp;E$1&amp;"'!$A$1:$P$33"))))&amp;"")</f>
-        <v>244</v>
+        <v>360</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -13370,7 +13370,6 @@
       <c r="B606" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13380,7 +13379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
@@ -15971,7 +15970,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16297,7 +16296,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D18" s="3">
         <v>204</v>
@@ -16306,25 +16305,25 @@
         <v>206</v>
       </c>
       <c r="F18" s="3">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G18" s="2">
         <v>163</v>
       </c>
       <c r="H18" s="3">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="I18" s="2">
         <v>180</v>
       </c>
       <c r="J18" s="3">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="K18" s="2">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="L18" s="3">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="M18" s="2">
         <v>140</v>
@@ -16343,37 +16342,37 @@
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="13">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="D19" s="14">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="E19" s="13">
         <v>191</v>
       </c>
       <c r="F19" s="14">
-        <v>127</v>
+        <v>52</v>
       </c>
       <c r="G19" s="13">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H19" s="14">
         <v>149</v>
       </c>
       <c r="I19" s="13">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="J19" s="14">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K19" s="13">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="L19" s="14">
         <v>238</v>
       </c>
       <c r="M19" s="13">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="13">
@@ -16390,34 +16389,34 @@
         <v>189</v>
       </c>
       <c r="D20" s="14">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="E20" s="13">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="F20" s="14">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="G20" s="13">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="H20" s="14">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="I20" s="13">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="J20" s="14">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="K20" s="13">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="L20" s="14">
         <v>152</v>
       </c>
       <c r="M20" s="13">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="N20" s="14">
         <v>184</v>
@@ -16433,28 +16432,28 @@
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="15">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D21" s="16">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E21" s="15">
-        <v>133</v>
+        <v>36</v>
       </c>
       <c r="F21" s="16">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="G21" s="15">
         <v>233</v>
       </c>
       <c r="H21" s="16">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="I21" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J21" s="16">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="K21" s="15">
         <v>182</v>
@@ -16463,10 +16462,10 @@
         <v>169</v>
       </c>
       <c r="M21" s="15">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="N21" s="16">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="O21" s="15">
         <v>197</v>
@@ -16486,31 +16485,31 @@
         <v>147</v>
       </c>
       <c r="D22" s="12">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E22" s="11">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="F22" s="12">
         <v>161</v>
       </c>
       <c r="G22" s="11">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="H22" s="12">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="I22" s="11">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="J22" s="12">
-        <v>112</v>
+        <v>28</v>
       </c>
       <c r="K22" s="11">
-        <v>23</v>
+        <v>135</v>
       </c>
       <c r="L22" s="12">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="M22" s="11">
         <v>155</v>
@@ -16531,32 +16530,32 @@
         <v>211</v>
       </c>
       <c r="C23" s="13">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D23" s="14">
         <v>207</v>
       </c>
       <c r="E23" s="13">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="F23" s="14">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="G23" s="13">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="H23" s="14">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="I23" s="13">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J23" s="14"/>
       <c r="K23" s="13">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="L23" s="14">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="M23" s="13">
         <v>136</v>
@@ -16579,31 +16578,31 @@
         <v>148</v>
       </c>
       <c r="E24" s="13">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="F24" s="14">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G24" s="13">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="H24" s="14">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="I24" s="13">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="J24" s="14">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="K24" s="13">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="L24" s="14">
         <v>186</v>
       </c>
       <c r="M24" s="13">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="N24" s="14">
         <v>141</v>
@@ -16631,22 +16630,22 @@
         <v>179</v>
       </c>
       <c r="G25" s="15">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="H25" s="16">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="I25" s="15">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J25" s="16">
-        <v>128</v>
+        <v>43</v>
       </c>
       <c r="K25" s="15">
         <v>150</v>
       </c>
       <c r="L25" s="16">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="M25" s="15">
         <v>181</v>
@@ -16658,7 +16657,7 @@
         <v>156</v>
       </c>
       <c r="P25" s="16">
-        <v>14</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -16672,37 +16671,37 @@
         <v>158</v>
       </c>
       <c r="D26" s="12">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="E26" s="11">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F26" s="12">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="G26" s="11">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="H26" s="12">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="I26" s="11">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="J26" s="12">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="K26" s="11">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="L26" s="12">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="M26" s="11">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="N26" s="12">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="O26" s="11">
         <v>210</v>
@@ -16722,16 +16721,16 @@
         <v>176</v>
       </c>
       <c r="D27" s="14">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E27" s="13">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="F27" s="14">
         <v>146</v>
       </c>
       <c r="G27" s="13">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="H27" s="14">
         <v>164</v>
@@ -16740,16 +16739,16 @@
         <v>237</v>
       </c>
       <c r="J27" s="14">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="K27" s="13">
         <v>183</v>
       </c>
       <c r="L27" s="14">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="M27" s="13">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="N27" s="14">
         <v>222</v>
@@ -16775,25 +16774,25 @@
         <v>166</v>
       </c>
       <c r="E28" s="13">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F28" s="14">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G28" s="13">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="H28" s="14">
         <v>236</v>
       </c>
       <c r="I28" s="13">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="J28" s="14">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="K28" s="13">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="L28" s="14">
         <v>137</v>
@@ -16822,37 +16821,37 @@
         <v>192</v>
       </c>
       <c r="D29" s="16">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="E29" s="15">
         <v>162</v>
       </c>
       <c r="F29" s="16">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G29" s="15">
         <v>165</v>
       </c>
       <c r="H29" s="16">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="I29" s="15">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="J29" s="16">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="K29" s="15">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="L29" s="16">
         <v>138</v>
       </c>
       <c r="M29" s="15">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="N29" s="16">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="O29" s="15">
         <v>195</v>
@@ -16875,34 +16874,34 @@
         <v>145</v>
       </c>
       <c r="E30" s="11">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="F30" s="12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G30" s="11">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="H30" s="12">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="I30" s="11">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="J30" s="12">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="K30" s="11">
         <v>209</v>
       </c>
       <c r="L30" s="12">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="M30" s="11">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="N30" s="12">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="O30" s="11">
         <v>153</v>
@@ -16919,40 +16918,40 @@
         <v>193</v>
       </c>
       <c r="C31" s="13">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="D31" s="14">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="E31" s="13">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F31" s="14">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G31" s="13">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="H31" s="14">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="I31" s="13">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J31" s="14">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="K31" s="13">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="L31" s="14">
         <v>151</v>
       </c>
       <c r="M31" s="13">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="N31" s="14">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="O31" s="13">
         <v>139</v>
@@ -16972,22 +16971,22 @@
         <v>143</v>
       </c>
       <c r="D32" s="14">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E32" s="13">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F32" s="14">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G32" s="13">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="H32" s="14">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="I32" s="13">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="J32" s="14">
         <v>17</v>
@@ -16996,10 +16995,10 @@
         <v>194</v>
       </c>
       <c r="L32" s="14">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="M32" s="13">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="N32" s="14">
         <v>168</v>
@@ -17022,43 +17021,43 @@
         <v>159</v>
       </c>
       <c r="D33" s="16">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E33" s="15">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F33" s="16">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="G33" s="15">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="H33" s="16">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="I33" s="15">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="J33" s="16">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="K33" s="15">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="L33" s="16">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M33" s="15">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="N33" s="16">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="O33" s="15">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="P33" s="16">
-        <v>35</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -17073,7 +17072,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Use naming scheme without Guard Ring for new probe card
</commit_message>
<xml_diff>
--- a/maps/SwitchBoardMapping.xlsx
+++ b/maps/SwitchBoardMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cern.ch\dfs\Users\e\esicking\Desktop\Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esicking\ProbecardNew\HGCAL_sensor_tests\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Probe card HPK 6in 256cells" sheetId="6" r:id="rId4"/>
     <sheet name="Probe card HPK 8in" sheetId="4" r:id="rId5"/>
     <sheet name="Probe card IFX 8in" sheetId="5" r:id="rId6"/>
-    <sheet name="Probe card 8in 199cells" sheetId="7" r:id="rId7"/>
+    <sheet name="Probe card 8in 198cells" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -59,7 +59,7 @@
     <t>/eos/user/h/hgsensor/HGCAL test results/Design/Probecard/HPK 6in 128ch/EDA-03517-V1-0_sch.pdf</t>
   </si>
   <si>
-    <t>Probe card 8in 199cells</t>
+    <t>Probe card 8in 198cells</t>
   </si>
 </sst>
 </file>
@@ -423,15 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,6 +440,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -849,7 +849,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F26" sqref="F26"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,27 +885,27 @@
     </row>
     <row r="2" spans="1:10" s="19" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
-        <f>SUMPRODUCT(NOT(ISBLANK(A$3:A$1000))*1)-COUNTIF(A$3:A$1000,"=#VALUE!")</f>
+        <f t="shared" ref="A2:F2" si="0">SUMPRODUCT(NOT(ISBLANK(A$3:A$1000))*1)-COUNTIF(A$3:A$1000,"=#VALUE!")</f>
         <v>599</v>
       </c>
       <c r="B2" s="19">
-        <f ca="1">SUMPRODUCT(NOT(ISBLANK(B$3:B$1000))*1)-COUNTIF(B$3:B$1000,"=#VALUE!")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>143</v>
       </c>
       <c r="C2" s="19">
-        <f ca="1">SUMPRODUCT(NOT(ISBLANK(C$3:C$1000))*1)-COUNTIF(C$3:C$1000,"=#VALUE!")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>280</v>
       </c>
       <c r="D2" s="19">
-        <f ca="1">SUMPRODUCT(NOT(ISBLANK(D$3:D$1000))*1)-COUNTIF(D$3:D$1000,"=#VALUE!")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>246</v>
       </c>
       <c r="E2" s="19">
-        <f ca="1">SUMPRODUCT(NOT(ISBLANK(E$3:E$1000))*1)-COUNTIF(E$3:E$1000,"=#VALUE!")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>248</v>
       </c>
       <c r="F2" s="19">
-        <f ca="1">SUMPRODUCT(NOT(ISBLANK(F$3:F$1000))*1)-COUNTIF(F$3:F$1000,"=#VALUE!")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>207</v>
       </c>
     </row>
@@ -15918,24 +15918,24 @@
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -17562,25 +17562,25 @@
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="37" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Probe card HPK 6in</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -18508,25 +18508,25 @@
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="37" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Probe card HPK 6in 256cells</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -19629,25 +19629,25 @@
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="37" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Probe card HPK 8in</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -20811,25 +20811,25 @@
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="37" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Probe card IFX 8in</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -21919,31 +21919,31 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="str">
+      <c r="A1" s="37" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
-        <v>Probe card 8in 199cells</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
+        <v>Probe card 8in 198cells</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
@@ -22242,14 +22242,14 @@
       <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="12"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
       <c r="K18" s="11"/>
@@ -22260,9 +22260,9 @@
       <c r="P18" s="12"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="14"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -22286,9 +22286,9 @@
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="14"/>
       <c r="E20" s="13"/>
       <c r="F20" s="14"/>
@@ -22312,9 +22312,9 @@
       <c r="P20" s="14"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="31"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="16"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>

</xml_diff>